<commit_message>
Update The Excel Sheet - Add new data to it
</commit_message>
<xml_diff>
--- a/Zero.xlsx
+++ b/Zero.xlsx
@@ -16,6 +16,71 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>cd</t>
+  </si>
+  <si>
+    <t>mkdir</t>
+  </si>
+  <si>
+    <t>لإنشاء مجلد في المسار الحالي</t>
+  </si>
+  <si>
+    <t>mkdir name-of-folder</t>
+  </si>
+  <si>
+    <t>للوصول الى المجلد root للجهاز او للوصول الى مسار محدد</t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>git clone any-path</t>
+  </si>
+  <si>
+    <t>cd OR cd any-path</t>
+  </si>
+  <si>
+    <t>نسخ المستودع الذي تم تحديدة في المسار الى المسار الحالي</t>
+  </si>
+  <si>
+    <t>dir</t>
+  </si>
+  <si>
+    <t>يقوم بأستعراض الملفات الموجودة في المسار الحالي</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>يوضح حالة working dirctory وماذا يوجد بها من تغييرات</t>
+  </si>
+  <si>
+    <t>git add</t>
+  </si>
+  <si>
+    <t>git add * OR git add name_file _in_working_dirctory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git reset head </t>
+  </si>
+  <si>
+    <t>[git reset head name_file] OR [git restore --staged name_file]</t>
+  </si>
+  <si>
+    <t>نقل الملفات من working dirctory الى staging area</t>
+  </si>
+  <si>
+    <t>التراجع عن الملفات التي في منطقة staging area وارجاعها الى منطقة working dirctory</t>
+  </si>
+  <si>
+    <t>git commit -m "msg-text"</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -331,12 +396,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified The Css File And Zero File
</commit_message>
<xml_diff>
--- a/Zero.xlsx
+++ b/Zero.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>cd</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>git commit -m "msg-text"</t>
+  </si>
+  <si>
+    <t>git branch</t>
+  </si>
+  <si>
+    <t>لمعرفة التفرعات الموجودة وماهو التفرع الحالي</t>
+  </si>
+  <si>
+    <t>git remote -v</t>
+  </si>
+  <si>
+    <t>لمعرفة اسم remote</t>
+  </si>
+  <si>
+    <t>git push origin master</t>
+  </si>
+  <si>
+    <t>لرفع التغيرات من الفرع master في الجهاز المحلي(local) الى origin في الجهاز البعيد (remote)</t>
   </si>
 </sst>
 </file>
@@ -396,17 +414,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
     <col min="2" max="2" width="55.28515625" customWidth="1"/>
-    <col min="3" max="3" width="67.28515625" customWidth="1"/>
+    <col min="3" max="3" width="69.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,6 +503,30 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>